<commit_message>
feat: elective planning excel
</commit_message>
<xml_diff>
--- a/misc/Electives Planning Index.xlsx
+++ b/misc/Electives Planning Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MTech\BITS-Software-engineering\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F89E4E-80DB-411E-8FE4-7263EA647A1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D74DDB9-7855-4310-8894-6CBDF5BA25F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="Z_B5432F8C_E6FB_4D99_B528_17825E16B3E5_.wvu.FilterData" localSheetId="0" hidden="1">Electives!$A$1:$Z$26</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
   <customWorkbookViews>
     <customWorkbookView name="Filter 1" guid="{B5432F8C-E6FB-4D99-B528-17825E16B3E5}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
   <si>
     <t>Course</t>
   </si>
@@ -132,34 +132,6 @@
   </si>
   <si>
     <t>SERVICE ORIENTED COMPUTING</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">It is the paradigm for distributed computing to enable application networks to be built using services as fundamental elements for developing applications. The aim of Service-Oriented Computing &amp; Applications is to publish original and high quality research results on the service-oriented computing (SOC) paradigm, models and technologies that have significant contributions to the advancement of service oriented systems and their applications.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Pre-requisites:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> Basic Programming, SOAP, Application of REST Architecture</t>
-    </r>
   </si>
   <si>
     <t>SE ZG583</t>
@@ -910,6 +882,29 @@
   <si>
     <t>Comment</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It is the paradigm for distributed computing to enable application networks to be built using services as fundamental elements for developing applications. The aim of Service-Oriented Computing &amp; Applications is to publish original and high quality research results on the service-oriented computing (SOC) paradigm, models and technologies that have significant contributions to the advancement of service oriented systems and their applications.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Pre-requisites:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> Basic Programming, SOAP, Application of REST Architecture</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1328,6 +1323,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:I26" dataDxfId="9">
+  <autoFilter ref="A1:I26" xr:uid="{A98AADAD-DA4E-4597-B190-46DF8895B848}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Course" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="7"/>
@@ -1543,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1589,7 +1585,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1670,7 +1666,9 @@
         <v>11</v>
       </c>
       <c r="H3" s="10"/>
-      <c r="I3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1703,7 +1701,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -1729,10 +1727,10 @@
     </row>
     <row r="5" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>2</v>
@@ -1741,14 +1739,16 @@
         <v>5</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1769,10 +1769,10 @@
     </row>
     <row r="6" spans="1:26" ht="40.799999999999997" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>2</v>
@@ -1781,14 +1781,16 @@
         <v>4</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="10"/>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1809,10 +1811,10 @@
     </row>
     <row r="7" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>2</v>
@@ -1821,14 +1823,16 @@
         <v>5</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1849,10 +1853,10 @@
     </row>
     <row r="8" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>2</v>
@@ -1861,14 +1865,16 @@
         <v>4</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1889,10 +1895,10 @@
     </row>
     <row r="9" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>2</v>
@@ -1901,7 +1907,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -1927,10 +1933,10 @@
     </row>
     <row r="10" spans="1:26" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>2</v>
@@ -1939,7 +1945,7 @@
         <v>4</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -1965,17 +1971,17 @@
     </row>
     <row r="11" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8">
         <v>3</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
@@ -2001,17 +2007,17 @@
     </row>
     <row r="12" spans="1:26" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8">
         <v>3</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -2037,17 +2043,17 @@
     </row>
     <row r="13" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8">
         <v>3</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -2073,17 +2079,17 @@
     </row>
     <row r="14" spans="1:26" ht="110.4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8">
         <v>5</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
@@ -2109,17 +2115,17 @@
     </row>
     <row r="15" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8">
         <v>4</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
@@ -2145,23 +2151,23 @@
     </row>
     <row r="16" spans="1:26" ht="81.599999999999994" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8">
         <v>5</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2183,23 +2189,23 @@
     </row>
     <row r="17" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8">
         <v>5</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -2221,17 +2227,17 @@
     </row>
     <row r="18" spans="1:26" ht="69.599999999999994" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8">
         <v>5</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
@@ -2257,17 +2263,17 @@
     </row>
     <row r="19" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8">
         <v>4</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
@@ -2293,17 +2299,17 @@
     </row>
     <row r="20" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8">
         <v>5</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
@@ -2329,17 +2335,17 @@
     </row>
     <row r="21" spans="1:26" ht="84" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8">
         <v>5</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
@@ -2365,17 +2371,17 @@
     </row>
     <row r="22" spans="1:26" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8">
         <v>4</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
@@ -2401,24 +2407,26 @@
     </row>
     <row r="23" spans="1:26" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10">
         <v>4</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I23" s="7"/>
+      <c r="I23" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -2439,23 +2447,23 @@
     </row>
     <row r="24" spans="1:26" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8">
         <v>4</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -2477,17 +2485,17 @@
     </row>
     <row r="25" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8">
         <v>5</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
@@ -2513,23 +2521,23 @@
     </row>
     <row r="26" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8">
         <v>4</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>

</xml_diff>